<commit_message>
Patching the autotransformer HT short-circuit current results, updating the test case.
git-svn-id: https://svn.code.sf.net/p/electricdss/code/trunk@3230 d8739450-1e93-4ef4-a0af-c327d92816ff
</commit_message>
<xml_diff>
--- a/Test/AutoTrans/AutoTest.xlsx
+++ b/Test/AutoTrans/AutoTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\OpenDSS\Test\AutoTrans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37C9920-CA94-47AE-A145-72E5814746B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E28FA95-9122-4C4F-86DF-944BAD3D1696}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9171" yWindow="2271" windowWidth="13140" windowHeight="14923" activeTab="1" xr2:uid="{36A0A5CE-3EE9-4EFC-A77C-7EADF4F78C50}"/>
+    <workbookView xWindow="16106" yWindow="1757" windowWidth="13140" windowHeight="14923" activeTab="1" xr2:uid="{36A0A5CE-3EE9-4EFC-A77C-7EADF4F78C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t>Winding</t>
   </si>
@@ -302,10 +302,7 @@
     <t>2. The two Dommel transformer models have a "natural" separation in load loss values of HT and LT, like the test report does.</t>
   </si>
   <si>
-    <t>3. Check the built-in AutoTrans for discrepancies in Isc-HT, and the load losses.</t>
-  </si>
-  <si>
-    <t>4. The built-in AutoTrans does match Isc-HL, core loss, and voltage regulation without the Dommel conversion.</t>
+    <t>3. The built-in AutoTrans matches test results without the Dommel conversion. It does not explicitly show the smaller MVA size.</t>
   </si>
 </sst>
 </file>
@@ -319,7 +316,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,23 +355,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -434,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -490,12 +473,11 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1708,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADFE9EB-33B2-479A-AFBD-EC6289AA7B21}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1774,8 +1756,8 @@
       <c r="D3" s="44">
         <v>2253.5500000000002</v>
       </c>
-      <c r="E3" s="46">
-        <v>2753.68</v>
+      <c r="E3" s="47">
+        <v>2253.44</v>
       </c>
       <c r="F3" s="23">
         <v>2258.6999999999998</v>
@@ -1795,7 +1777,7 @@
         <v>4152.54</v>
       </c>
       <c r="E4" s="44">
-        <v>4151.7700000000004</v>
+        <v>4151.3599999999997</v>
       </c>
       <c r="F4" s="23">
         <v>4159.5</v>
@@ -1814,8 +1796,8 @@
       <c r="D5" s="44">
         <v>348.78</v>
       </c>
-      <c r="E5" s="46">
-        <v>-153600</v>
+      <c r="E5" s="47">
+        <v>348.959</v>
       </c>
       <c r="F5" s="23">
         <v>346.2</v>
@@ -1834,8 +1816,8 @@
       <c r="D6" s="44">
         <v>223.53899999999999</v>
       </c>
-      <c r="E6" s="46">
-        <v>-33473.555</v>
+      <c r="E6" s="47">
+        <v>223.428</v>
       </c>
       <c r="F6" s="23">
         <v>225.8</v>
@@ -1855,7 +1837,7 @@
         <v>240.298</v>
       </c>
       <c r="E7" s="47">
-        <v>318.33269999999999</v>
+        <v>239.07300000000001</v>
       </c>
       <c r="F7" s="23">
         <v>246.4</v>
@@ -1970,7 +1952,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="46" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1987,11 +1969,6 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>